<commit_message>
Modified mock excel file
</commit_message>
<xml_diff>
--- a/Assets/mock_data.xlsx
+++ b/Assets/mock_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Questions and Polyfills</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>What are the supported access points?</t>
+  </si>
+  <si>
+    <t>Instant APs</t>
+  </si>
+  <si>
+    <t>iaps.htm</t>
+  </si>
+  <si>
+    <t>What are instant APs?</t>
+  </si>
+  <si>
+    <t>define Instant APs</t>
+  </si>
+  <si>
+    <t>What are IAPs?</t>
+  </si>
+  <si>
+    <t>Define IAPs</t>
   </si>
 </sst>
 </file>
@@ -151,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="data_table" displayName="data_table" ref="A1:D21">
-  <autoFilter ref="A1:D21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="data_table" displayName="data_table" ref="A1:D26">
+  <autoFilter ref="A1:D26">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -431,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +589,40 @@
         <v>23</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>